<commit_message>
Updating per last update with more information
</commit_message>
<xml_diff>
--- a/Submittal Automation - Testing/BLANK_MISC/Key Personnel List.xlsx
+++ b/Submittal Automation - Testing/BLANK_MISC/Key Personnel List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BCST-352-BH\Documents\Higashi_Files\Useful\Submittal Automation\Misc Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BCST-414\Documents\Higashi_Files\Useful\BCS Programming\Submittal Automation-v0.201602017\BLANK_MISC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,25 +53,25 @@
     <t>BICSI ITS Technician</t>
   </si>
   <si>
-    <t>808-782-8884</t>
-  </si>
-  <si>
-    <t>ryan@bcshawaii.com</t>
-  </si>
-  <si>
     <t>KEY PERSONNEL</t>
   </si>
   <si>
     <t>Yokoi, David R.</t>
   </si>
   <si>
-    <t>Yokoi, Ryan K.</t>
-  </si>
-  <si>
     <t>ADDRESS</t>
   </si>
   <si>
     <t>LONG</t>
+  </si>
+  <si>
+    <t>Tandal, Mason M.</t>
+  </si>
+  <si>
+    <t>808-722-7257</t>
+  </si>
+  <si>
+    <t>mason.tandal@bcshawaii.com</t>
   </si>
 </sst>
 </file>
@@ -280,19 +280,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -436,6 +423,21 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -449,7 +451,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -461,19 +463,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -483,49 +479,52 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -835,7 +834,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,95 +842,95 @@
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
+      <c r="A1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28"/>
+      <c r="A2" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="25"/>
+      <c r="A3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="11"/>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="9" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
+      <c r="B5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
+      <c r="B6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>